<commit_message>
regression results appeared; winner minus loser appeared
</commit_message>
<xml_diff>
--- a/output_testing_t-test_result.xlsx
+++ b/output_testing_t-test_result.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,12 +484,20 @@
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>arbitrage</t>
+          <t>loser_minus_winner</t>
         </is>
       </c>
       <c r="M1" s="1" t="n"/>
       <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>winner_minus_loser</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -563,6 +571,26 @@
           <t>symbol</t>
         </is>
       </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>acar</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>t_stat</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -611,6 +639,16 @@
         <v>0.3534513907020555</v>
       </c>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>-0.006218138045699179</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1.095274689453224</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.3534513907020555</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -652,6 +690,16 @@
         <v>0.4385168181670432</v>
       </c>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>-0.00712044838380254</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.8911165443441785</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.4385168181670432</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -693,6 +741,16 @@
         <v>0.3079685848069909</v>
       </c>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>-0.009764388525428323</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1.225049238800761</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.3079685848069909</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -734,6 +792,16 @@
         <v>0.5596251730802592</v>
       </c>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>-0.006216175304906462</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-0.6542613644017724</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.5596251730802592</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -775,6 +843,16 @@
         <v>0.8693259841663411</v>
       </c>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>-0.001960684145158755</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-0.1790252582612103</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.8693259841663411</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -816,6 +894,16 @@
         <v>0.8743244734401874</v>
       </c>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>-0.001975357945848453</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-0.1720851215551122</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.8743244734401874</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -857,6 +945,16 @@
         <v>0.868932999629038</v>
       </c>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>0.002519954251120355</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.1795713734141034</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.868932999629038</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -898,6 +996,16 @@
         <v>0.8073144632389374</v>
       </c>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>0.004741822968728761</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.2662255980285859</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.8073144632389374</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -939,6 +1047,16 @@
         <v>0.8129163145323867</v>
       </c>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" t="n">
+        <v>0.00512205272220346</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.2582517252428179</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.8129163145323867</v>
+      </c>
+      <c r="S12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -980,6 +1098,16 @@
         <v>0.9342638252401354</v>
       </c>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" t="n">
+        <v>0.001509490001515477</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.08958355190114456</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.9342638252401354</v>
+      </c>
+      <c r="S13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1021,6 +1149,16 @@
         <v>0.5938399774004647</v>
       </c>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>0.0105797237513938</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.5948241335958523</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.5938399774004647</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1062,6 +1200,16 @@
         <v>0.5752044518384947</v>
       </c>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" t="n">
+        <v>0.01224467376228971</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.6268739019901524</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.5752044518384947</v>
+      </c>
+      <c r="S15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1103,6 +1251,16 @@
         <v>0.6434412929079893</v>
       </c>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" t="n">
+        <v>0.01024900426904687</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.5128337311871574</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.6434412929079893</v>
+      </c>
+      <c r="S16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1144,6 +1302,16 @@
         <v>0.455204925898847</v>
       </c>
       <c r="O17" t="inlineStr"/>
+      <c r="P17" t="n">
+        <v>0.01718130104800336</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.8554071305204506</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.455204925898847</v>
+      </c>
+      <c r="S17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1185,6 +1353,16 @@
         <v>0.4382928377374748</v>
       </c>
       <c r="O18" t="inlineStr"/>
+      <c r="P18" t="n">
+        <v>0.01787972313662934</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.8916039970447464</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.4382928377374748</v>
+      </c>
+      <c r="S18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1226,6 +1404,16 @@
         <v>0.3467208124382281</v>
       </c>
       <c r="O19" t="inlineStr"/>
+      <c r="P19" t="n">
+        <v>0.02238607938999151</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1.113387588151705</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.3467208124382281</v>
+      </c>
+      <c r="S19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1267,6 +1455,16 @@
         <v>0.3243487645952166</v>
       </c>
       <c r="O20" t="inlineStr"/>
+      <c r="P20" t="n">
+        <v>0.02248954194317506</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1.176211912752152</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.3243487645952166</v>
+      </c>
+      <c r="S20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1308,6 +1506,16 @@
         <v>0.2305301168147705</v>
       </c>
       <c r="O21" t="inlineStr"/>
+      <c r="P21" t="n">
+        <v>0.02703628434178373</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1.50022394840083</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.2305301168147705</v>
+      </c>
+      <c r="S21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1349,6 +1557,16 @@
         <v>0.238101557275725</v>
       </c>
       <c r="O22" t="inlineStr"/>
+      <c r="P22" t="n">
+        <v>0.02388837030168869</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1.4692277058128</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.238101557275725</v>
+      </c>
+      <c r="S22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1390,10 +1608,21 @@
         <v>0.2359231599186822</v>
       </c>
       <c r="O23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>0.02121371741746491</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1.478033960904889</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.2359231599186822</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
   </mergeCells>
@@ -1407,7 +1636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,12 +1666,20 @@
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>arbitrage</t>
+          <t>loser_minus_winner</t>
         </is>
       </c>
       <c r="M1" s="1" t="n"/>
       <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>winner_minus_loser</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="n"/>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -1516,6 +1753,26 @@
           <t>symbol</t>
         </is>
       </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>acar</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>t_stat</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1564,6 +1821,16 @@
         <v>0.3319581239790347</v>
       </c>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="n">
+        <v>-0.03277045410971666</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1.154369321019939</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.3319581239790347</v>
+      </c>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1605,6 +1872,16 @@
         <v>0.2299688145496731</v>
       </c>
       <c r="O5" t="inlineStr"/>
+      <c r="P5" t="n">
+        <v>-0.04161430299547681</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1.502566103927719</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.2299688145496731</v>
+      </c>
+      <c r="S5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1646,6 +1923,16 @@
         <v>0.1859455575130352</v>
       </c>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" t="n">
+        <v>-0.04641086549033971</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1.709199394014179</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.1859455575130352</v>
+      </c>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1687,6 +1974,16 @@
         <v>0.09446201525304078</v>
       </c>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" t="n">
+        <v>-0.05820740649147691</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-2.416531787335073</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.09446201525304078</v>
+      </c>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1728,6 +2025,16 @@
         <v>0.07474629575614075</v>
       </c>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
+        <v>-0.06105748898178266</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-2.684754395254032</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.07474629575614075</v>
+      </c>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1769,6 +2076,16 @@
         <v>0.08270273262924596</v>
       </c>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" t="n">
+        <v>-0.06437591322125974</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-2.567081834470976</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.08270273262924596</v>
+      </c>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1810,6 +2127,16 @@
         <v>0.05316677162160148</v>
       </c>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" t="n">
+        <v>-0.06791416787412376</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-3.10309973500109</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.05316677162160148</v>
+      </c>
+      <c r="S10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1851,6 +2178,16 @@
         <v>0.05640514786405077</v>
       </c>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" t="n">
+        <v>-0.06524426884969045</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-3.027890767217726</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.05640514786405077</v>
+      </c>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1896,6 +2233,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P12" t="n">
+        <v>-0.06593709560200915</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-3.182976295400078</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.04997965988528884</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1941,6 +2292,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P13" t="n">
+        <v>-0.06984935636785702</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-3.465469104526848</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.04047914179629381</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1982,6 +2347,16 @@
         <v>0.0558917009931375</v>
       </c>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" t="n">
+        <v>-0.05665193198207794</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-3.039447752465818</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.0558917009931375</v>
+      </c>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2027,6 +2402,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P15" t="n">
+        <v>-0.0593783624199701</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-3.252088044496669</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.0474145120116711</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2072,6 +2461,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P16" t="n">
+        <v>-0.0568238954851378</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-3.74121441842017</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.03331673204326352</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2117,6 +2520,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P17" t="n">
+        <v>-0.06485215083133977</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-4.125695972580717</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.02582178580412216</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2162,6 +2579,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P18" t="n">
+        <v>-0.07034812292352144</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-4.998813205004021</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.01540245733561628</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2207,6 +2638,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P19" t="n">
+        <v>-0.06929573822159087</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-5.366968719751083</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.01266201889991631</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2252,6 +2697,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P20" t="n">
+        <v>-0.0685759510798344</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>-4.889119142745103</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.01636641087868123</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2297,6 +2756,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P21" t="n">
+        <v>-0.06074917089821999</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>-3.887621601485423</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.03016925796841825</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2342,6 +2815,20 @@
           <t>*</t>
         </is>
       </c>
+      <c r="P22" t="n">
+        <v>-0.05866200943814983</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-3.339228654994927</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.04441294921426441</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2383,10 +2870,21 @@
         <v>0.0864968367402319</v>
       </c>
       <c r="O23" t="inlineStr"/>
+      <c r="P23" t="n">
+        <v>-0.05368848821226194</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-2.515779932154497</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.0864968367402319</v>
+      </c>
+      <c r="S23" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
   </mergeCells>

</xml_diff>